<commit_message>
Changed data for column failure/advisory items qai comments
</commit_message>
<xml_diff>
--- a/src/resources/retro_report_template.xlsx
+++ b/src/resources/retro_report_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oalexandru/workspace/cvs-tsk-retro-gen/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D98D2CB5-2C6F-234C-9D2C-72F0F9023B85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3C6C04-A467-9F45-96D4-6662D58DAA5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34240" yWindow="1200" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -839,12 +839,30 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -853,24 +871,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1195,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1259,13 +1259,13 @@
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="28"/>
       <c r="E4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="28"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
@@ -1278,14 +1278,14 @@
     </row>
     <row r="5" spans="1:16" s="1" customFormat="1" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="23"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="28"/>
       <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
@@ -1301,13 +1301,13 @@
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="23"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -1323,13 +1323,13 @@
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="23"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
@@ -1383,13 +1383,13 @@
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="23"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
@@ -1405,13 +1405,13 @@
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="28"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
@@ -1427,13 +1427,13 @@
       <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="23"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="28"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
@@ -1446,14 +1446,14 @@
     </row>
     <row r="13" spans="1:16" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="32"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
@@ -1546,18 +1546,18 @@
     </row>
     <row r="17" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
       <c r="P17" s="12"/>
@@ -1781,16 +1781,16 @@
     </row>
     <row r="30" spans="1:16" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="30" t="s">
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="31"/>
-      <c r="G30" s="32"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="26"/>
       <c r="H30" s="16"/>
       <c r="I30" s="16"/>
       <c r="J30" s="16"/>
@@ -1803,12 +1803,12 @@
     </row>
     <row r="31" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="32"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="26"/>
       <c r="H31" s="16"/>
       <c r="I31" s="16"/>
       <c r="J31" s="16"/>
@@ -1862,17 +1862,17 @@
       <c r="B34" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="32"/>
+      <c r="D34" s="26"/>
       <c r="E34" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F34" s="30" t="s">
+      <c r="F34" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="32"/>
+      <c r="G34" s="26"/>
       <c r="H34" s="16"/>
       <c r="I34" s="16"/>
       <c r="J34" s="16"/>
@@ -1886,11 +1886,11 @@
     <row r="35" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="5"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="29"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="23"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="29"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="23"/>
       <c r="H35" s="16"/>
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
@@ -1975,6 +1975,21 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="F35:G35"/>
     <mergeCell ref="B30:D30"/>
@@ -1983,21 +1998,6 @@
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="F34:G34"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed other formatting stuff
</commit_message>
<xml_diff>
--- a/src/resources/retro_report_template.xlsx
+++ b/src/resources/retro_report_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oalexandru/workspace/cvs-tsk-retro-gen/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A605D02-C163-9040-8366-F979F5EC49A2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9297F01A-82DE-184C-A1ED-D89264FCB6AB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36180" yWindow="2280" windowWidth="33600" windowHeight="18940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Retrokey report template TO BE" sheetId="1" r:id="rId1"/>
@@ -280,20 +280,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
@@ -306,6 +292,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -488,7 +486,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -733,6 +731,15 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -780,19 +787,45 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -805,70 +838,60 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1193,787 +1216,796 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="57.5" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="0.1640625" customWidth="1"/>
-    <col min="5" max="5" width="39.1640625" customWidth="1"/>
-    <col min="6" max="6" width="37.6640625" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" customWidth="1"/>
-    <col min="8" max="8" width="20.5" customWidth="1"/>
-    <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="26.1640625" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" customWidth="1"/>
-    <col min="12" max="12" width="26.83203125" customWidth="1"/>
-    <col min="13" max="13" width="53.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="15"/>
+    <col min="2" max="2" width="57.5" style="15" customWidth="1"/>
+    <col min="3" max="3" width="18" style="15" customWidth="1"/>
+    <col min="4" max="4" width="0.1640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="39.1640625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="37.6640625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="20.5" style="15" customWidth="1"/>
+    <col min="9" max="9" width="16" style="15" customWidth="1"/>
+    <col min="10" max="10" width="26.1640625" style="15" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" style="15" customWidth="1"/>
+    <col min="12" max="12" width="26.83203125" style="15" customWidth="1"/>
+    <col min="13" max="13" width="53.6640625" style="15" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="38" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="8"/>
-    </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10" t="s">
+    <row r="1" spans="1:16" ht="38" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="2" spans="1:16" ht="20" x14ac:dyDescent="0.2">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="18"/>
+    </row>
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="11"/>
-    </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="4" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="6"/>
+    </row>
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="4" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="11"/>
-    </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="4" t="s">
+      <c r="F4" s="33"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="6"/>
+    </row>
+    <row r="5" spans="1:16" s="1" customFormat="1" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="11"/>
-    </row>
-    <row r="6" spans="1:16" s="1" customFormat="1" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
-      <c r="B6" s="4" t="s">
+      <c r="F5" s="33"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="6"/>
+    </row>
+    <row r="6" spans="1:16" s="1" customFormat="1" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="4" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="11"/>
-    </row>
-    <row r="7" spans="1:16" s="1" customFormat="1" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="4" t="s">
+      <c r="F6" s="33"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="6"/>
+    </row>
+    <row r="7" spans="1:16" s="1" customFormat="1" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="4" t="s">
+      <c r="C7" s="33"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="11"/>
-    </row>
-    <row r="8" spans="1:16" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="11"/>
-    </row>
-    <row r="9" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="20" t="s">
+      <c r="F7" s="33"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="6"/>
+    </row>
+    <row r="8" spans="1:16" s="1" customFormat="1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A8" s="19"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="6"/>
+    </row>
+    <row r="9" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="11"/>
-    </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="4" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="6"/>
+    </row>
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="4" t="s">
+      <c r="C10" s="33"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="27"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="11"/>
-    </row>
-    <row r="11" spans="1:16" s="1" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="4" t="s">
+      <c r="F10" s="33"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="6"/>
+    </row>
+    <row r="11" spans="1:16" s="1" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="4" t="s">
+      <c r="C11" s="33"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="11"/>
-    </row>
-    <row r="12" spans="1:16" s="1" customFormat="1" ht="73" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="4" t="s">
+      <c r="F11" s="33"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="6"/>
+    </row>
+    <row r="12" spans="1:16" s="1" customFormat="1" ht="73" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="4" t="s">
+      <c r="C12" s="33"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="11"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="6"/>
     </row>
     <row r="13" spans="1:16" s="2" customFormat="1" ht="50" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="29" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="14"/>
-    </row>
-    <row r="14" spans="1:16" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="11"/>
-    </row>
-    <row r="15" spans="1:16" s="1" customFormat="1" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10" t="s">
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="8"/>
+    </row>
+    <row r="14" spans="1:16" s="1" customFormat="1" ht="20" x14ac:dyDescent="0.2">
+      <c r="A14" s="19"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="6"/>
+    </row>
+    <row r="15" spans="1:16" s="1" customFormat="1" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="11"/>
-    </row>
-    <row r="16" spans="1:16" s="1" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="4" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="6"/>
+    </row>
+    <row r="16" spans="1:16" s="1" customFormat="1" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="M16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="11"/>
-    </row>
-    <row r="17" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="11"/>
-    </row>
-    <row r="18" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="16"/>
-    </row>
-    <row r="19" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="16"/>
-    </row>
-    <row r="20" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="16"/>
-    </row>
-    <row r="21" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="16"/>
-    </row>
-    <row r="22" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="16"/>
-    </row>
-    <row r="23" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="16"/>
-    </row>
-    <row r="24" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="16"/>
-    </row>
-    <row r="25" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="16"/>
-    </row>
-    <row r="26" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
-      <c r="P26" s="16"/>
-    </row>
-    <row r="27" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="16"/>
-    </row>
-    <row r="28" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="16"/>
-    </row>
-    <row r="29" spans="1:16" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
-      <c r="B29" s="10" t="s">
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="6"/>
+    </row>
+    <row r="17" spans="1:16" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="6"/>
+    </row>
+    <row r="18" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="22"/>
+    </row>
+    <row r="19" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="22"/>
+    </row>
+    <row r="20" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="22"/>
+    </row>
+    <row r="21" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="22"/>
+    </row>
+    <row r="22" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="22"/>
+    </row>
+    <row r="23" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="22"/>
+    </row>
+    <row r="24" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="19"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="22"/>
+    </row>
+    <row r="25" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="22"/>
+    </row>
+    <row r="26" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="22"/>
+    </row>
+    <row r="27" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="19"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="22"/>
+    </row>
+    <row r="28" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="19"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="22"/>
+    </row>
+    <row r="29" spans="1:16" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="19"/>
+      <c r="B29" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="16"/>
-    </row>
-    <row r="30" spans="1:16" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="24" t="s">
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="22"/>
+    </row>
+    <row r="30" spans="1:16" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
+      <c r="B30" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="24" t="s">
+      <c r="C30" s="29"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="25"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="16"/>
-    </row>
-    <row r="31" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="16"/>
-    </row>
-    <row r="32" spans="1:16" ht="44" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="16"/>
-    </row>
-    <row r="33" spans="1:16" s="3" customFormat="1" ht="58" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
-      <c r="B33" s="10" t="s">
+      <c r="F30" s="29"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="22"/>
+    </row>
+    <row r="31" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="22"/>
+    </row>
+    <row r="32" spans="1:16" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="19"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="22"/>
+    </row>
+    <row r="33" spans="1:16" s="23" customFormat="1" ht="58" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="19"/>
+      <c r="B33" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15"/>
-      <c r="N33" s="15"/>
-      <c r="O33" s="15"/>
-      <c r="P33" s="16"/>
-    </row>
-    <row r="34" spans="1:16" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
-      <c r="B34" s="4" t="s">
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="22"/>
+    </row>
+    <row r="34" spans="1:16" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="19"/>
+      <c r="B34" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="4" t="s">
+      <c r="D34" s="14"/>
+      <c r="E34" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F34" s="24" t="s">
+      <c r="F34" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="26"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="15"/>
-      <c r="P34" s="16"/>
-    </row>
-    <row r="35" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="16"/>
-    </row>
-    <row r="36" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="16"/>
-    </row>
-    <row r="37" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="15"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
-      <c r="P37" s="16"/>
-    </row>
-    <row r="38" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="16"/>
-    </row>
-    <row r="39" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="19"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="22"/>
+    </row>
+    <row r="35" spans="1:16" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="19"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="22"/>
+    </row>
+    <row r="36" spans="1:16" ht="20" x14ac:dyDescent="0.2">
+      <c r="A36" s="19"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="22"/>
+    </row>
+    <row r="37" spans="1:16" ht="20" x14ac:dyDescent="0.2">
+      <c r="A37" s="19"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="22"/>
+    </row>
+    <row r="38" spans="1:16" ht="20" x14ac:dyDescent="0.2">
+      <c r="A38" s="19"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="22"/>
+    </row>
+    <row r="39" spans="1:16" ht="20" x14ac:dyDescent="0.2">
+      <c r="A39" s="26"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+      <c r="K39" s="24"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="24"/>
+      <c r="N39" s="24"/>
+      <c r="O39" s="24"/>
+      <c r="P39" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="C6:D6"/>
@@ -1982,13 +2014,6 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F7:G7"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>